<commit_message>
It's not the Qpoint voltage that's brought out to Vneg, it's the Raw_Neg_Voltage.  Update the documentation and calculator to reflect this reality.
</commit_message>
<xml_diff>
--- a/Tube_Audio/Helper_Circuits/EFB_Bias_Supply/EFB_Bias_Supply_Calculator.xlsx
+++ b/Tube_Audio/Helper_Circuits/EFB_Bias_Supply/EFB_Bias_Supply_Calculator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="460" windowWidth="28800" windowHeight="16680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>Input Raw_Neg_Voltage at rectifier here:</t>
   </si>
   <si>
-    <t>Vin</t>
-  </si>
-  <si>
     <t>Target_Qpoint_Voltage_Drop:</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>R5</t>
   </si>
   <si>
-    <t>Qpoint_Voltage (Vneg):</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">This value should be roughly double of the target </t>
     </r>
@@ -396,6 +390,12 @@
   </si>
   <si>
     <t>best results, measure.</t>
+  </si>
+  <si>
+    <t>Vneg</t>
+  </si>
+  <si>
+    <t>Qpoint_Voltage:</t>
   </si>
 </sst>
 </file>
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -790,32 +790,32 @@
         <v>475</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="E3" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="E4" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
       <c r="E5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H5" s="8">
         <f>(B2/0.00075)/2</f>
         <v>316666.66666666669</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J5" s="8">
         <f>B2-(B2*(H6/(H5+H6)))</f>
@@ -825,14 +825,14 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H6" s="8">
         <f>(B2/0.00075)/2</f>
         <v>316666.66666666669</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J6" s="8">
         <f>B2-J5</f>
@@ -842,7 +842,7 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H7" s="8">
         <f>H5+H6</f>
@@ -851,7 +851,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -864,7 +864,7 @@
       </c>
       <c r="E10" s="6"/>
       <c r="I10" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J10" s="8">
         <f>B2-(B2*(B11/(B10+B11)))</f>
@@ -880,7 +880,7 @@
       </c>
       <c r="E11" s="6"/>
       <c r="I11" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J11" s="8">
         <f>B2-J10</f>
@@ -911,7 +911,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H14" s="10"/>
     </row>
@@ -923,18 +923,18 @@
         <v>-63</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E16" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E17" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H17" s="8">
         <f>((0-B15)/H12)-(H19/2)</f>
@@ -1044,21 +1044,21 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B38" s="3">
         <v>0</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1067,11 +1067,11 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B40" s="5"/>
       <c r="E40" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H40" s="11">
         <f>0-(B41*1.4)</f>
@@ -1080,29 +1080,29 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B41" s="3">
         <v>120</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E42" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B43" s="5"/>
       <c r="E43" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E44" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1110,7 +1110,7 @@
         <v>21</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H46" s="8">
         <f>0-(B47-(2*B15))</f>
@@ -1119,28 +1119,28 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B47" s="3">
         <v>-168</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E48" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E49" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E51" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H51" s="8">
         <f>H46/(H35+B38)</f>
@@ -1149,20 +1149,20 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E52" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E53" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="H55" s="8">
         <f>B47-(0-(H35*B56))</f>
@@ -1171,28 +1171,28 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B56" s="3">
         <v>6800</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E57" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E58" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E60" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H60" s="8">
         <f>(H55)-(B15)/H30</f>
@@ -1201,20 +1201,20 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E61" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E62" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="H64" s="8">
         <f>(0-(H55-B15))/B65</f>
@@ -1223,28 +1223,28 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B65" s="3">
         <v>43000</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E66" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E67" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -1276,7 +1276,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B73">
         <f>B65</f>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B74">
         <f>B56</f>
@@ -1294,12 +1294,12 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B77">
         <f>H25</f>

</xml_diff>

<commit_message>
Use the resistance of the "Individul_Bias_Network" simulation as the Rnetwork resistance in the calculator example.
</commit_message>
<xml_diff>
--- a/Tube_Audio/Helper_Circuits/EFB_Bias_Supply/EFB_Bias_Supply_Calculator.xlsx
+++ b/Tube_Audio/Helper_Circuits/EFB_Bias_Supply/EFB_Bias_Supply_Calculator.xlsx
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="H32" s="8">
         <f>(0-B15)/B33</f>
-        <v>4.1999999999999997E-3</v>
+        <v>3.8769230769230769E-3</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1027,7 +1027,7 @@
         <v>18</v>
       </c>
       <c r="B33" s="3">
-        <v>15000</v>
+        <v>16250</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="H35" s="8">
         <f>H12+H30+H32</f>
-        <v>6.4196969696969693E-3</v>
+        <v>6.0966200466200469E-3</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="H51" s="8">
         <f>H46/(H35+B38)</f>
-        <v>6542.364880811896</v>
+        <v>6889.0630675409584</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="H55" s="8">
         <f>B47-(0-(H35*B56))</f>
-        <v>-124.3460606060606</v>
+        <v>-126.54298368298367</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="H60" s="8">
         <f>(H55)-(B15)/H30</f>
-        <v>41875.653939393938</v>
+        <v>41873.457016317014</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="H64" s="8">
         <f>(0-(H55-B15))/B65</f>
-        <v>1.4266525722339675E-3</v>
+        <v>1.4777438065810156E-3</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>